<commit_message>
้history log แสดง no data ซ้ำ
</commit_message>
<xml_diff>
--- a/public/customer_report.xlsx
+++ b/public/customer_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>ตู้เข้า</t>
   </si>
@@ -50,55 +50,25 @@
     <t>email</t>
   </si>
   <si>
-    <t xml:space="preserve">ร่ำรวย จำกัด (ชลุบรี) </t>
-  </si>
-  <si>
-    <t>จริงใจ มั่นคง</t>
-  </si>
-  <si>
-    <t>067-467-4532</t>
-  </si>
-  <si>
-    <t>jingjai@gmail.com</t>
-  </si>
-  <si>
-    <t>สยามโปรดักซ์</t>
-  </si>
-  <si>
-    <t>กฤษ รุ่งเจริญ</t>
-  </si>
-  <si>
-    <t>087-056-0356</t>
-  </si>
-  <si>
-    <t>kirst2534@gmail.com</t>
-  </si>
-  <si>
-    <t>Kingtons</t>
-  </si>
-  <si>
-    <t>อรธิชา รุ่งเรือง</t>
-  </si>
-  <si>
-    <t>087-567-8945</t>
-  </si>
-  <si>
-    <t>ornticha@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">อรุณ ฟาร์ม (กรุงเทพ) </t>
-  </si>
-  <si>
-    <t>ณัฐกรณ์ สุขใจ</t>
-  </si>
-  <si>
-    <t>064-234-5678</t>
-  </si>
-  <si>
-    <t>natthakorn@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betagro (กรุงเทพ) </t>
+    <t>วิรัตน์ สากร</t>
+  </si>
+  <si>
+    <t>083-081-7901</t>
+  </si>
+  <si>
+    <t>wirat00@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ซัน จำกัด (ศรีราชา) </t>
+  </si>
+  <si>
+    <t>083-081-7900</t>
+  </si>
+  <si>
+    <t>wirativ@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At Pro Solution (กรุงเทพ) </t>
   </si>
   <si>
     <t>สุวยุทธ เยาวจิต</t>
@@ -110,16 +80,34 @@
     <t>suwayuth@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">ไอวี (แสนสุข) </t>
-  </si>
-  <si>
-    <t>วิรัตน์ สากร</t>
-  </si>
-  <si>
-    <t>083-081-7916</t>
-  </si>
-  <si>
-    <t>wirativ@gmail.com</t>
+    <t>ทดสอบ</t>
+  </si>
+  <si>
+    <t>wirat@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At Pro Solution (ศรีราชา) </t>
+  </si>
+  <si>
+    <t>วสันต์ ทัดแก้ว</t>
+  </si>
+  <si>
+    <t>087-567-8959</t>
+  </si>
+  <si>
+    <t>ornticha9@gmail.com</t>
+  </si>
+  <si>
+    <t>เจ พลัส</t>
+  </si>
+  <si>
+    <t>วิรัตน์000 สากร000</t>
+  </si>
+  <si>
+    <t>083-081-7000</t>
+  </si>
+  <si>
+    <t>wirat000@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -538,11 +526,11 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="9.10" style="1"/>
-    <col min="2" max="2" width="39" bestFit="true" customWidth="true" style="2"/>
-    <col min="3" max="3" width="28" bestFit="true" customWidth="true" style="1"/>
+    <col min="2" max="2" width="45" bestFit="true" customWidth="true" style="2"/>
+    <col min="3" max="3" width="32" bestFit="true" customWidth="true" style="1"/>
     <col min="4" max="4" width="38" bestFit="true" customWidth="true" style="1"/>
     <col min="5" max="5" width="36" bestFit="true" customWidth="true" style="1"/>
-    <col min="6" max="6" width="35" bestFit="true" customWidth="true" style="1"/>
+    <col min="6" max="6" width="33" bestFit="true" customWidth="true" style="1"/>
     <col min="7" max="7" width="9.10" style="1"/>
     <col min="8" max="8" width="9.10" style="1"/>
     <col min="9" max="9" width="9.10" style="1"/>
@@ -570,13 +558,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -584,13 +572,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -598,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
@@ -629,101 +617,101 @@
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="B10" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D10" s="8">
         <v>0</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="B11" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D11" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="B12" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D12" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>